<commit_message>
Release 1.0.1 BETA (mobile friendly and status bar added)
</commit_message>
<xml_diff>
--- a/MAYO.xlsx
+++ b/MAYO.xlsx
@@ -475,59 +475,59 @@
   </sheetPr>
   <dimension ref="A1:J15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5:J11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="2" t="inlineStr">
+      <c r="A1" s="3" t="inlineStr">
         <is>
           <t>Job#</t>
         </is>
       </c>
-      <c r="B1" s="2" t="inlineStr">
+      <c r="B1" s="3" t="inlineStr">
         <is>
           <t>Loc.</t>
         </is>
       </c>
-      <c r="C1" s="2" t="inlineStr">
+      <c r="C1" s="3" t="inlineStr">
         <is>
           <t>Tasks</t>
         </is>
       </c>
-      <c r="D1" s="2" t="inlineStr">
+      <c r="D1" s="3" t="inlineStr">
         <is>
           <t>Bal Date</t>
         </is>
       </c>
-      <c r="E1" s="2" t="inlineStr">
+      <c r="E1" s="3" t="inlineStr">
         <is>
           <t>Com Date</t>
         </is>
       </c>
-      <c r="F1" s="2" t="inlineStr">
+      <c r="F1" s="3" t="inlineStr">
         <is>
           <t>Install</t>
         </is>
       </c>
-      <c r="G1" s="2" t="inlineStr">
+      <c r="G1" s="3" t="inlineStr">
         <is>
           <t>Tech</t>
         </is>
       </c>
-      <c r="H1" s="2" t="inlineStr">
+      <c r="H1" s="3" t="inlineStr">
         <is>
           <t>Design</t>
         </is>
       </c>
-      <c r="I1" s="2" t="inlineStr">
+      <c r="I1" s="3" t="inlineStr">
         <is>
           <t>Lead</t>
         </is>
       </c>
-      <c r="J1" s="2" t="inlineStr">
+      <c r="J1" s="3" t="inlineStr">
         <is>
           <t>Last Modified</t>
         </is>
@@ -536,7 +536,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>ABAM</t>
+          <t>ABAM2</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -547,6 +547,17 @@
       <c r="C2" t="inlineStr">
         <is>
           <t>MRG EP Demo</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr"/>
+      <c r="E2" t="inlineStr"/>
+      <c r="F2" t="inlineStr"/>
+      <c r="G2" t="inlineStr"/>
+      <c r="H2" t="inlineStr"/>
+      <c r="I2" t="inlineStr"/>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>Issac Magallanes</t>
         </is>
       </c>
     </row>
@@ -566,6 +577,13 @@
           <t>Demo Phase Roush-in 8/23 |  Setra Low Tap (Temp'd for now) | Adair Install</t>
         </is>
       </c>
+      <c r="D3" t="inlineStr"/>
+      <c r="E3" t="inlineStr"/>
+      <c r="F3" t="inlineStr"/>
+      <c r="G3" t="inlineStr"/>
+      <c r="H3" t="inlineStr"/>
+      <c r="I3" t="inlineStr"/>
+      <c r="J3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -583,6 +601,13 @@
           <t>Verify, Nurse Call: CX 8/20-8/24</t>
         </is>
       </c>
+      <c r="D4" t="inlineStr"/>
+      <c r="E4" t="inlineStr"/>
+      <c r="F4" t="inlineStr"/>
+      <c r="G4" t="inlineStr"/>
+      <c r="H4" t="inlineStr"/>
+      <c r="I4" t="inlineStr"/>
+      <c r="J4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -600,6 +625,13 @@
           <t>Generose - Graphic, Controller Naming | Tom / Adair</t>
         </is>
       </c>
+      <c r="D5" t="inlineStr"/>
+      <c r="E5" t="inlineStr"/>
+      <c r="F5" t="inlineStr"/>
+      <c r="G5" t="inlineStr"/>
+      <c r="H5" t="inlineStr"/>
+      <c r="I5" t="inlineStr"/>
+      <c r="J5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -617,6 +649,13 @@
           <t>RR demo - check back 8/22 | FCU Steam Vlv at office</t>
         </is>
       </c>
+      <c r="D6" t="inlineStr"/>
+      <c r="E6" t="inlineStr"/>
+      <c r="F6" t="inlineStr"/>
+      <c r="G6" t="inlineStr"/>
+      <c r="H6" t="inlineStr"/>
+      <c r="I6" t="inlineStr"/>
+      <c r="J6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -634,6 +673,13 @@
           <t>VAV/FCU ready for Point checkout, 9 VAV, 1 FCU, 8 F/s, 2 Hx, 1 O2 Seas, 1 Duct Sens</t>
         </is>
       </c>
+      <c r="D7" t="inlineStr"/>
+      <c r="E7" t="inlineStr"/>
+      <c r="F7" t="inlineStr"/>
+      <c r="G7" t="inlineStr"/>
+      <c r="H7" t="inlineStr"/>
+      <c r="I7" t="inlineStr"/>
+      <c r="J7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -651,6 +697,13 @@
           <t>MR-34</t>
         </is>
       </c>
+      <c r="D8" t="inlineStr"/>
+      <c r="E8" t="inlineStr"/>
+      <c r="F8" t="inlineStr"/>
+      <c r="G8" t="inlineStr"/>
+      <c r="H8" t="inlineStr"/>
+      <c r="I8" t="inlineStr"/>
+      <c r="J8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -668,6 +721,13 @@
           <t>Chiller 1.2_FEC-006 Head-End Clean-up</t>
         </is>
       </c>
+      <c r="D9" t="inlineStr"/>
+      <c r="E9" t="inlineStr"/>
+      <c r="F9" t="inlineStr"/>
+      <c r="G9" t="inlineStr"/>
+      <c r="H9" t="inlineStr"/>
+      <c r="I9" t="inlineStr"/>
+      <c r="J9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -685,6 +745,13 @@
           <t>Locker Rooms</t>
         </is>
       </c>
+      <c r="D10" t="inlineStr"/>
+      <c r="E10" t="inlineStr"/>
+      <c r="F10" t="inlineStr"/>
+      <c r="G10" t="inlineStr"/>
+      <c r="H10" t="inlineStr"/>
+      <c r="I10" t="inlineStr"/>
+      <c r="J10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -702,6 +769,13 @@
           <t>FS-8 AFMS Install</t>
         </is>
       </c>
+      <c r="D11" t="inlineStr"/>
+      <c r="E11" t="inlineStr"/>
+      <c r="F11" t="inlineStr"/>
+      <c r="G11" t="inlineStr"/>
+      <c r="H11" t="inlineStr"/>
+      <c r="I11" t="inlineStr"/>
+      <c r="J11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -719,6 +793,13 @@
           <t>11 Vlvs + 6 T-Stats Demo</t>
         </is>
       </c>
+      <c r="D12" t="inlineStr"/>
+      <c r="E12" t="inlineStr"/>
+      <c r="F12" t="inlineStr"/>
+      <c r="G12" t="inlineStr"/>
+      <c r="H12" t="inlineStr"/>
+      <c r="I12" t="inlineStr"/>
+      <c r="J12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -736,6 +817,13 @@
           <t>Keeping Open</t>
         </is>
       </c>
+      <c r="D13" t="inlineStr"/>
+      <c r="E13" t="inlineStr"/>
+      <c r="F13" t="inlineStr"/>
+      <c r="G13" t="inlineStr"/>
+      <c r="H13" t="inlineStr"/>
+      <c r="I13" t="inlineStr"/>
+      <c r="J13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -783,6 +871,7 @@
           <t>Submit RFI</t>
         </is>
       </c>
+      <c r="J14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -800,21 +889,25 @@
           <t>General Notes 2</t>
         </is>
       </c>
+      <c r="D15" t="inlineStr"/>
       <c r="E15" t="inlineStr">
         <is>
           <t>10/2</t>
         </is>
       </c>
+      <c r="F15" t="inlineStr"/>
       <c r="G15" t="inlineStr">
         <is>
           <t>VAV Checkout</t>
         </is>
       </c>
+      <c r="H15" t="inlineStr"/>
       <c r="I15" t="inlineStr">
         <is>
           <t>Submit RFI</t>
         </is>
       </c>
+      <c r="J15" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -903,13 +996,6 @@
           <t>FC Bus Download/Vout</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr"/>
-      <c r="E2" t="inlineStr"/>
-      <c r="F2" t="inlineStr"/>
-      <c r="G2" t="inlineStr"/>
-      <c r="H2" t="inlineStr"/>
-      <c r="I2" t="inlineStr"/>
-      <c r="J2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -927,13 +1013,6 @@
           <t>Condensate pump replacement</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr"/>
-      <c r="E3" t="inlineStr"/>
-      <c r="F3" t="inlineStr"/>
-      <c r="G3" t="inlineStr"/>
-      <c r="H3" t="inlineStr"/>
-      <c r="I3" t="inlineStr"/>
-      <c r="J3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -946,14 +1025,6 @@
           <t>Ei07-3</t>
         </is>
       </c>
-      <c r="C4" t="inlineStr"/>
-      <c r="D4" t="inlineStr"/>
-      <c r="E4" t="inlineStr"/>
-      <c r="F4" t="inlineStr"/>
-      <c r="G4" t="inlineStr"/>
-      <c r="H4" t="inlineStr"/>
-      <c r="I4" t="inlineStr"/>
-      <c r="J4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -971,13 +1042,6 @@
           <t>Replace Steam Coil</t>
         </is>
       </c>
-      <c r="D5" t="inlineStr"/>
-      <c r="E5" t="inlineStr"/>
-      <c r="F5" t="inlineStr"/>
-      <c r="G5" t="inlineStr"/>
-      <c r="H5" t="inlineStr"/>
-      <c r="I5" t="inlineStr"/>
-      <c r="J5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -995,13 +1059,6 @@
           <t>Replace Iso Dmp; some night after 10 pm</t>
         </is>
       </c>
-      <c r="D6" t="inlineStr"/>
-      <c r="E6" t="inlineStr"/>
-      <c r="F6" t="inlineStr"/>
-      <c r="G6" t="inlineStr"/>
-      <c r="H6" t="inlineStr"/>
-      <c r="I6" t="inlineStr"/>
-      <c r="J6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -1019,13 +1076,6 @@
           <t>Wet Filter DP's!</t>
         </is>
       </c>
-      <c r="D7" t="inlineStr"/>
-      <c r="E7" t="inlineStr"/>
-      <c r="F7" t="inlineStr"/>
-      <c r="G7" t="inlineStr"/>
-      <c r="H7" t="inlineStr"/>
-      <c r="I7" t="inlineStr"/>
-      <c r="J7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -1043,13 +1093,6 @@
           <t>EFI Iso Dampers</t>
         </is>
       </c>
-      <c r="D8" t="inlineStr"/>
-      <c r="E8" t="inlineStr"/>
-      <c r="F8" t="inlineStr"/>
-      <c r="G8" t="inlineStr"/>
-      <c r="H8" t="inlineStr"/>
-      <c r="I8" t="inlineStr"/>
-      <c r="J8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -1067,13 +1110,6 @@
           <t>Pipe/Device VAVs</t>
         </is>
       </c>
-      <c r="D9" t="inlineStr"/>
-      <c r="E9" t="inlineStr"/>
-      <c r="F9" t="inlineStr"/>
-      <c r="G9" t="inlineStr"/>
-      <c r="H9" t="inlineStr"/>
-      <c r="I9" t="inlineStr"/>
-      <c r="J9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -1091,13 +1127,6 @@
           <t>Fix piping for North side F/S Dampers, Rough-In, Stat relocates</t>
         </is>
       </c>
-      <c r="D10" t="inlineStr"/>
-      <c r="E10" t="inlineStr"/>
-      <c r="F10" t="inlineStr"/>
-      <c r="G10" t="inlineStr"/>
-      <c r="H10" t="inlineStr"/>
-      <c r="I10" t="inlineStr"/>
-      <c r="J10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -1115,13 +1144,6 @@
           <t>Material Only</t>
         </is>
       </c>
-      <c r="D11" t="inlineStr"/>
-      <c r="E11" t="inlineStr"/>
-      <c r="F11" t="inlineStr"/>
-      <c r="G11" t="inlineStr"/>
-      <c r="H11" t="inlineStr"/>
-      <c r="I11" t="inlineStr"/>
-      <c r="J11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -1139,13 +1161,6 @@
           <t>JB S-105A, JB S-105B, Ei58, EiR8</t>
         </is>
       </c>
-      <c r="D12" t="inlineStr"/>
-      <c r="E12" t="inlineStr"/>
-      <c r="F12" t="inlineStr"/>
-      <c r="G12" t="inlineStr"/>
-      <c r="H12" t="inlineStr"/>
-      <c r="I12" t="inlineStr"/>
-      <c r="J12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -1163,13 +1178,6 @@
           <t>FC + N2 Clean-up, wire valves, upgrade between VAV</t>
         </is>
       </c>
-      <c r="D13" t="inlineStr"/>
-      <c r="E13" t="inlineStr"/>
-      <c r="F13" t="inlineStr"/>
-      <c r="G13" t="inlineStr"/>
-      <c r="H13" t="inlineStr"/>
-      <c r="I13" t="inlineStr"/>
-      <c r="J13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -1187,13 +1195,6 @@
           <t>Cx 9/26</t>
         </is>
       </c>
-      <c r="D14" t="inlineStr"/>
-      <c r="E14" t="inlineStr"/>
-      <c r="F14" t="inlineStr"/>
-      <c r="G14" t="inlineStr"/>
-      <c r="H14" t="inlineStr"/>
-      <c r="I14" t="inlineStr"/>
-      <c r="J14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -1211,13 +1212,6 @@
           <t>Facilities Shot | Panel: Relocate/Writing</t>
         </is>
       </c>
-      <c r="D15" t="inlineStr"/>
-      <c r="E15" t="inlineStr"/>
-      <c r="F15" t="inlineStr"/>
-      <c r="G15" t="inlineStr"/>
-      <c r="H15" t="inlineStr"/>
-      <c r="I15" t="inlineStr"/>
-      <c r="J15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -1235,13 +1229,6 @@
           <t>Cx</t>
         </is>
       </c>
-      <c r="D16" t="inlineStr"/>
-      <c r="E16" t="inlineStr"/>
-      <c r="F16" t="inlineStr"/>
-      <c r="G16" t="inlineStr"/>
-      <c r="H16" t="inlineStr"/>
-      <c r="I16" t="inlineStr"/>
-      <c r="J16" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Release 1.3.0 BETA (Reorder Job Func)
</commit_message>
<xml_diff>
--- a/MAYO.xlsx
+++ b/MAYO.xlsx
@@ -1,39 +1,50 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="3720" yWindow="500" windowWidth="32120" windowHeight="20700" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="SMH" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="RMH" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="SMH" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="RMH" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="0" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1" refMode="A1" iterate="0" iterateCount="100" iterateDelta="0.0001"/>
 </workbook>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="4">
+  <fonts count="6">
     <font>
       <name val="Calibri"/>
+      <charset val="1"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <b val="1"/>
+      <color rgb="FF000000"/>
       <sz val="11"/>
     </font>
     <font>
-      <name val="Calibri"/>
-      <family val="2"/>
+      <name val="Arial"/>
+      <family val="0"/>
+      <sz val="10"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <family val="0"/>
+      <sz val="10"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <family val="0"/>
+      <sz val="10"/>
+    </font>
+    <font>
+      <name val="Cambria"/>
+      <charset val="1"/>
+      <family val="0"/>
       <b val="1"/>
       <sz val="11"/>
     </font>
@@ -49,7 +60,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -58,33 +69,10 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
       <diagonal/>
     </border>
     <border>
@@ -94,25 +82,45 @@
       <bottom style="thin"/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="6">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1">
+      <alignment horizontal="general" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+  <cellXfs count="7">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="general" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="general" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="general" vertical="bottom"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="2" builtinId="6"/>
+    <cellStyle name="Currency" xfId="3" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="4" builtinId="7"/>
+    <cellStyle name="Percent" xfId="5" builtinId="5"/>
   </cellStyles>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="00000000"/>
@@ -536,7 +544,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>ABAM2</t>
+          <t>ABAM</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -612,7 +620,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>4-319</t>
+          <t>4-0319</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -670,7 +678,7 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>VAV/FCU ready for Point checkout, 9 VAV, 1 FCU, 8 F/s, 2 Hx, 1 O2 Seas, 1 Duct Sens</t>
+          <t>VAV/FCU ready for Point checkout, 9 VAV, 1 FCU, 8 F/s, 2 Hx, 1 O2 Sens, 1 Duct Sens</t>
         </is>
       </c>
       <c r="D7" t="inlineStr"/>
@@ -679,7 +687,11 @@
       <c r="G7" t="inlineStr"/>
       <c r="H7" t="inlineStr"/>
       <c r="I7" t="inlineStr"/>
-      <c r="J7" t="inlineStr"/>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>Issac Magallanes</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -780,17 +792,17 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>4-0385</t>
+          <t>4-0073</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Brach03</t>
+          <t>Al03</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>11 Vlvs + 6 T-Stats Demo</t>
+          <t>Keeping Open</t>
         </is>
       </c>
       <c r="D12" t="inlineStr"/>
@@ -804,110 +816,118 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>4-0073</t>
+          <t>4-0520</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Al03</t>
+          <t>Mb05 East Tower</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Keeping Open</t>
-        </is>
-      </c>
-      <c r="D13" t="inlineStr"/>
-      <c r="E13" t="inlineStr"/>
-      <c r="F13" t="inlineStr"/>
-      <c r="G13" t="inlineStr"/>
-      <c r="H13" t="inlineStr"/>
-      <c r="I13" t="inlineStr"/>
-      <c r="J13" t="inlineStr"/>
+          <t>Mb05 East Fit Up. Rough-In starts 10/14.</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>Jul 2025</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>Aug 2025</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>Adair-Walk Through 6 F/S Damper. 16 Pt Rm VAV's, 14 normal VAV's, 24 RadVlvs. Rough-in starts 10/14</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>Checkout-Months. Initial Walk-through, site investigation</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>Order Material, submittal: HUM VLV</t>
+        </is>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Walk Through </t>
+        </is>
+      </c>
+      <c r="J13" t="inlineStr">
+        <is>
+          <t>Issac Magallanes</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Test</t>
+          <t>4-0490</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Building</t>
+          <t>Mh4-5-7</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>General Notes 2</t>
-        </is>
-      </c>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t>9/30</t>
-        </is>
-      </c>
-      <c r="E14" t="inlineStr">
-        <is>
-          <t>10/2</t>
-        </is>
-      </c>
+          <t>Cons of MH: Pneumatic Demo on Marion 4-5-7. Bakken Project</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr"/>
+      <c r="E14" t="inlineStr"/>
       <c r="F14" t="inlineStr">
         <is>
-          <t>Pipe and Install panel</t>
-        </is>
-      </c>
-      <c r="G14" t="inlineStr">
-        <is>
-          <t>VAV Checkout</t>
-        </is>
-      </c>
-      <c r="H14" t="inlineStr">
-        <is>
-          <t>Finish Redlines</t>
-        </is>
-      </c>
-      <c r="I14" t="inlineStr">
-        <is>
-          <t>Submit RFI</t>
-        </is>
-      </c>
-      <c r="J14" t="inlineStr"/>
+          <t xml:space="preserve">Demo </t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr"/>
+      <c r="H14" t="inlineStr"/>
+      <c r="I14" t="inlineStr"/>
+      <c r="J14" t="inlineStr">
+        <is>
+          <t>Tony Nigon</t>
+        </is>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Test</t>
+          <t>4-0522</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Building</t>
+          <t>Mh3-4</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>General Notes 2</t>
+          <t>MH 3-4th Fl Remodel Rasmussen Job</t>
         </is>
       </c>
       <c r="D15" t="inlineStr"/>
-      <c r="E15" t="inlineStr">
-        <is>
-          <t>10/2</t>
-        </is>
-      </c>
-      <c r="F15" t="inlineStr"/>
-      <c r="G15" t="inlineStr">
-        <is>
-          <t>VAV Checkout</t>
-        </is>
-      </c>
+      <c r="E15" t="inlineStr"/>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>Pnuematic Demo</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr"/>
       <c r="H15" t="inlineStr"/>
-      <c r="I15" t="inlineStr">
-        <is>
-          <t>Submit RFI</t>
-        </is>
-      </c>
-      <c r="J15" t="inlineStr"/>
+      <c r="I15" t="inlineStr"/>
+      <c r="J15" t="inlineStr">
+        <is>
+          <t>Tony Nigon</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -920,7 +940,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J16"/>
+  <dimension ref="A1:J27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -981,252 +1001,766 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
+      <c r="A2" s="6" t="inlineStr">
+        <is>
+          <t>3-0216</t>
+        </is>
+      </c>
+      <c r="B2" s="6" t="inlineStr">
+        <is>
+          <t>Ei07</t>
+        </is>
+      </c>
+      <c r="C2" s="6" t="inlineStr"/>
+      <c r="D2" s="6" t="inlineStr"/>
+      <c r="E2" s="6" t="inlineStr"/>
+      <c r="F2" s="6" t="inlineStr"/>
+      <c r="G2" s="6" t="inlineStr"/>
+      <c r="H2" s="6" t="inlineStr"/>
+      <c r="I2" s="6" t="inlineStr"/>
+      <c r="J2" s="6" t="inlineStr">
+        <is>
+          <t>Colton</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="6" t="inlineStr">
+        <is>
+          <t>3-0423</t>
+        </is>
+      </c>
+      <c r="B3" s="6" t="inlineStr">
+        <is>
+          <t>PTI Vibration</t>
+        </is>
+      </c>
+      <c r="C3" s="6" t="inlineStr">
+        <is>
+          <t>JBS-105A, JBS-105B, EIS-8, EIR-8</t>
+        </is>
+      </c>
+      <c r="D3" s="6" t="inlineStr"/>
+      <c r="E3" s="6" t="inlineStr"/>
+      <c r="F3" s="6" t="inlineStr"/>
+      <c r="G3" s="6" t="inlineStr"/>
+      <c r="H3" s="6" t="inlineStr"/>
+      <c r="I3" s="6" t="inlineStr"/>
+      <c r="J3" s="6" t="inlineStr">
+        <is>
+          <t>Colton</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="6" t="inlineStr">
+        <is>
+          <t>3-0435</t>
+        </is>
+      </c>
+      <c r="B4" s="6" t="inlineStr">
+        <is>
+          <t>Ei00S-MR1</t>
+        </is>
+      </c>
+      <c r="C4" s="6" t="inlineStr">
+        <is>
+          <t>Wet Filter DP's</t>
+        </is>
+      </c>
+      <c r="D4" s="6" t="inlineStr"/>
+      <c r="E4" s="6" t="inlineStr"/>
+      <c r="F4" s="6" t="inlineStr"/>
+      <c r="G4" s="6" t="inlineStr"/>
+      <c r="H4" s="6" t="inlineStr"/>
+      <c r="I4" s="6" t="inlineStr"/>
+      <c r="J4" s="6" t="inlineStr">
+        <is>
+          <t>Colton</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="6" t="inlineStr">
+        <is>
+          <t>4-0114</t>
+        </is>
+      </c>
+      <c r="B5" s="6" t="inlineStr">
+        <is>
+          <t>EiPH</t>
+        </is>
+      </c>
+      <c r="C5" s="6" t="inlineStr">
+        <is>
+          <t>EF-1 Iso Dampers</t>
+        </is>
+      </c>
+      <c r="D5" s="6" t="inlineStr"/>
+      <c r="E5" s="6" t="inlineStr"/>
+      <c r="F5" s="6" t="inlineStr"/>
+      <c r="G5" s="6" t="inlineStr"/>
+      <c r="H5" s="6" t="inlineStr"/>
+      <c r="I5" s="6" t="inlineStr"/>
+      <c r="J5" s="6" t="inlineStr">
+        <is>
+          <t>Colton</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="6" t="inlineStr">
+        <is>
+          <t>4-0201</t>
+        </is>
+      </c>
+      <c r="B6" s="6" t="inlineStr">
+        <is>
+          <t>Ch01</t>
+        </is>
+      </c>
+      <c r="C6" s="6" t="inlineStr">
+        <is>
+          <t>Download/checkout</t>
+        </is>
+      </c>
+      <c r="D6" s="6" t="inlineStr"/>
+      <c r="E6" s="6" t="inlineStr"/>
+      <c r="F6" s="6" t="inlineStr"/>
+      <c r="G6" s="6" t="inlineStr"/>
+      <c r="H6" s="6" t="inlineStr"/>
+      <c r="I6" s="6" t="inlineStr"/>
+      <c r="J6" s="6" t="inlineStr">
+        <is>
+          <t>Colton</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="6" t="inlineStr">
+        <is>
+          <t>4-0271</t>
+        </is>
+      </c>
+      <c r="B7" s="6" t="inlineStr">
+        <is>
+          <t>JB - Labor</t>
+        </is>
+      </c>
+      <c r="C7" s="6" t="inlineStr">
+        <is>
+          <t>Fix piping for North side F/S Dampers, Stat Relocates, Pipe/Device VAVs</t>
+        </is>
+      </c>
+      <c r="D7" s="6" t="inlineStr"/>
+      <c r="E7" s="6" t="inlineStr"/>
+      <c r="F7" s="6" t="inlineStr"/>
+      <c r="G7" s="6" t="inlineStr"/>
+      <c r="H7" s="6" t="inlineStr"/>
+      <c r="I7" s="6" t="inlineStr"/>
+      <c r="J7" s="6" t="inlineStr">
+        <is>
+          <t>Colton</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="6" t="inlineStr">
+        <is>
+          <t>4-0272</t>
+        </is>
+      </c>
+      <c r="B8" s="6" t="inlineStr">
+        <is>
+          <t>JB - Material</t>
+        </is>
+      </c>
+      <c r="C8" s="6" t="inlineStr">
+        <is>
+          <t>Material Only</t>
+        </is>
+      </c>
+      <c r="D8" s="6" t="inlineStr"/>
+      <c r="E8" s="6" t="inlineStr"/>
+      <c r="F8" s="6" t="inlineStr"/>
+      <c r="G8" s="6" t="inlineStr"/>
+      <c r="H8" s="6" t="inlineStr"/>
+      <c r="I8" s="6" t="inlineStr"/>
+      <c r="J8" s="6" t="inlineStr"/>
+    </row>
+    <row r="9">
+      <c r="A9" s="6" t="inlineStr">
+        <is>
+          <t>4-0277</t>
+        </is>
+      </c>
+      <c r="B9" s="6" t="inlineStr">
+        <is>
+          <t>Ch00S</t>
+        </is>
+      </c>
+      <c r="C9" s="6" t="inlineStr">
+        <is>
+          <t>Humidifier Install, F/S Dmp in Breakroom</t>
+        </is>
+      </c>
+      <c r="D9" s="6" t="inlineStr"/>
+      <c r="E9" s="6" t="inlineStr"/>
+      <c r="F9" s="6" t="inlineStr"/>
+      <c r="G9" s="6" t="inlineStr"/>
+      <c r="H9" s="6" t="inlineStr"/>
+      <c r="I9" s="6" t="inlineStr"/>
+      <c r="J9" s="6" t="inlineStr">
+        <is>
+          <t>Colton</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="6" t="inlineStr">
+        <is>
+          <t>4-0322</t>
+        </is>
+      </c>
+      <c r="B10" s="6" t="inlineStr">
+        <is>
+          <t>Ch01</t>
+        </is>
+      </c>
+      <c r="C10" s="6" t="inlineStr">
+        <is>
+          <t>Pipe/Device VAV</t>
+        </is>
+      </c>
+      <c r="D10" s="6" t="inlineStr"/>
+      <c r="E10" s="6" t="inlineStr"/>
+      <c r="F10" s="6" t="inlineStr"/>
+      <c r="G10" s="6" t="inlineStr"/>
+      <c r="H10" s="6" t="inlineStr"/>
+      <c r="I10" s="6" t="inlineStr"/>
+      <c r="J10" s="6" t="inlineStr">
+        <is>
+          <t>Colton</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="6" t="inlineStr">
+        <is>
+          <t>4-0350</t>
+        </is>
+      </c>
+      <c r="B11" s="6" t="inlineStr">
+        <is>
+          <t>Jb01</t>
+        </is>
+      </c>
+      <c r="C11" s="6" t="inlineStr">
+        <is>
+          <t>Leak Detection</t>
+        </is>
+      </c>
+      <c r="D11" s="6" t="inlineStr"/>
+      <c r="E11" s="6" t="inlineStr"/>
+      <c r="F11" s="6" t="inlineStr"/>
+      <c r="G11" s="6" t="inlineStr"/>
+      <c r="H11" s="6" t="inlineStr"/>
+      <c r="I11" s="6" t="inlineStr"/>
+      <c r="J11" s="6" t="inlineStr">
+        <is>
+          <t>Colton</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="6" t="inlineStr">
         <is>
           <t>4-0356</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr">
+      <c r="B12" s="6" t="inlineStr">
         <is>
           <t>Ei00L Cafeteria</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>FC Bus Download/Vout</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>3-0195</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>EI005</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>Condensate pump replacement</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>3-0216</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>Ei07-3</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
+      <c r="C12" s="6" t="inlineStr">
+        <is>
+          <t>Download/checkout</t>
+        </is>
+      </c>
+      <c r="D12" s="6" t="inlineStr"/>
+      <c r="E12" s="6" t="inlineStr"/>
+      <c r="F12" s="6" t="inlineStr"/>
+      <c r="G12" s="6" t="inlineStr"/>
+      <c r="H12" s="6" t="inlineStr"/>
+      <c r="I12" s="6" t="inlineStr"/>
+      <c r="J12" s="6" t="inlineStr">
+        <is>
+          <t>Colton</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="6" t="inlineStr">
+        <is>
+          <t>4-0391</t>
+        </is>
+      </c>
+      <c r="B13" s="6" t="inlineStr">
+        <is>
+          <t>Ei01-360</t>
+        </is>
+      </c>
+      <c r="C13" s="6" t="inlineStr">
+        <is>
+          <t>Install of new VAV - Adair</t>
+        </is>
+      </c>
+      <c r="D13" s="6" t="inlineStr"/>
+      <c r="E13" s="6" t="inlineStr"/>
+      <c r="F13" s="6" t="inlineStr"/>
+      <c r="G13" s="6" t="inlineStr"/>
+      <c r="H13" s="6" t="inlineStr"/>
+      <c r="I13" s="6" t="inlineStr"/>
+      <c r="J13" s="6" t="inlineStr">
+        <is>
+          <t>Colton</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="6" t="inlineStr">
+        <is>
+          <t>2-0120 (temp)</t>
+        </is>
+      </c>
+      <c r="B14" s="6" t="inlineStr">
+        <is>
+          <t>Gu19, Gu20, Al09</t>
+        </is>
+      </c>
+      <c r="C14" s="6" t="inlineStr">
+        <is>
+          <t>Demo phase 1 on Gu19 until 10/24.  NO JOB NUMBER YET. Status of Gug19?</t>
+        </is>
+      </c>
+      <c r="D14" s="6" t="inlineStr"/>
+      <c r="E14" s="6" t="inlineStr"/>
+      <c r="F14" s="6" t="inlineStr">
+        <is>
+          <t>Pneumatic Demo on Gug19 til 10/24. Phase 2 Alfred starts in Feb 2025</t>
+        </is>
+      </c>
+      <c r="G14" s="6" t="inlineStr"/>
+      <c r="H14" s="6" t="inlineStr"/>
+      <c r="I14" s="6" t="inlineStr">
+        <is>
+          <t>Dominate</t>
+        </is>
+      </c>
+      <c r="J14" s="6" t="inlineStr">
+        <is>
+          <t>Tony Nigon</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="6" t="inlineStr">
+        <is>
+          <t>4-0435</t>
+        </is>
+      </c>
+      <c r="B15" s="6" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Si11 </t>
+        </is>
+      </c>
+      <c r="C15" s="6" t="inlineStr">
+        <is>
+          <t>Project 4. Phase 2 starts 3/17/25</t>
+        </is>
+      </c>
+      <c r="D15" s="6" t="inlineStr"/>
+      <c r="E15" s="6" t="inlineStr"/>
+      <c r="F15" s="6" t="inlineStr">
+        <is>
+          <t>3/17/25 Phase 2</t>
+        </is>
+      </c>
+      <c r="G15" s="6" t="inlineStr"/>
+      <c r="H15" s="6" t="inlineStr"/>
+      <c r="I15" s="6" t="inlineStr"/>
+      <c r="J15" s="6" t="inlineStr">
+        <is>
+          <t>Tony Nigon</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="6" t="inlineStr">
+        <is>
+          <t>4-0440</t>
+        </is>
+      </c>
+      <c r="B16" s="6" t="inlineStr">
+        <is>
+          <t>Albert Lea ED</t>
+        </is>
+      </c>
+      <c r="C16" s="6" t="inlineStr">
+        <is>
+          <t>Pneumatic Demo, work starts in December (?)</t>
+        </is>
+      </c>
+      <c r="D16" s="6" t="inlineStr"/>
+      <c r="E16" s="6" t="inlineStr"/>
+      <c r="F16" s="6" t="inlineStr">
+        <is>
+          <t>Pneumatic demo</t>
+        </is>
+      </c>
+      <c r="G16" s="6" t="inlineStr"/>
+      <c r="H16" s="6" t="inlineStr"/>
+      <c r="I16" s="6" t="inlineStr"/>
+      <c r="J16" s="6" t="inlineStr">
+        <is>
+          <t>Tony Nigon</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="6" t="inlineStr">
+        <is>
+          <t>5-0473</t>
+        </is>
+      </c>
+      <c r="B17" s="6" t="inlineStr">
+        <is>
+          <t>Go15</t>
+        </is>
+      </c>
+      <c r="C17" s="6" t="inlineStr">
+        <is>
+          <t>New Procedure Room, pneumatic demo</t>
+        </is>
+      </c>
+      <c r="D17" s="6" t="inlineStr"/>
+      <c r="E17" s="6" t="inlineStr"/>
+      <c r="F17" s="6" t="inlineStr">
+        <is>
+          <t>demo</t>
+        </is>
+      </c>
+      <c r="G17" s="6" t="inlineStr"/>
+      <c r="H17" s="6" t="inlineStr"/>
+      <c r="I17" s="6" t="inlineStr"/>
+      <c r="J17" s="6" t="inlineStr">
+        <is>
+          <t>Tony Nigon</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="6" t="inlineStr">
+        <is>
+          <t>5-0478</t>
+        </is>
+      </c>
+      <c r="B18" s="6" t="inlineStr">
+        <is>
+          <t>Mayo 20/21</t>
+        </is>
+      </c>
+      <c r="C18" s="6" t="inlineStr">
+        <is>
+          <t>Demo of 1 AHU on each floor-Done?</t>
+        </is>
+      </c>
+      <c r="D18" s="6" t="inlineStr"/>
+      <c r="E18" s="6" t="inlineStr"/>
+      <c r="F18" s="6" t="inlineStr">
+        <is>
+          <t>Demo</t>
+        </is>
+      </c>
+      <c r="G18" s="6" t="inlineStr"/>
+      <c r="H18" s="6" t="inlineStr"/>
+      <c r="I18" s="6" t="inlineStr"/>
+      <c r="J18" s="6" t="inlineStr">
+        <is>
+          <t>Tony Nigon</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="6" t="inlineStr">
+        <is>
+          <t>4-0485</t>
+        </is>
+      </c>
+      <c r="B19" s="6" t="inlineStr">
+        <is>
+          <t>Ei00S-67 Facilities Shop</t>
+        </is>
+      </c>
+      <c r="C19" s="6" t="inlineStr">
+        <is>
+          <t>Cx</t>
+        </is>
+      </c>
+      <c r="D19" s="6" t="inlineStr"/>
+      <c r="E19" s="6" t="inlineStr"/>
+      <c r="F19" s="6" t="inlineStr"/>
+      <c r="G19" s="6" t="inlineStr"/>
+      <c r="H19" s="6" t="inlineStr"/>
+      <c r="I19" s="6" t="inlineStr"/>
+      <c r="J19" s="6" t="inlineStr">
+        <is>
+          <t>Colton</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="6" t="inlineStr">
+        <is>
+          <t>4-0526</t>
+        </is>
+      </c>
+      <c r="B20" s="6" t="inlineStr">
+        <is>
+          <t>Ch00S</t>
+        </is>
+      </c>
+      <c r="C20" s="6" t="inlineStr">
+        <is>
+          <t>MR-56 Starts 11/4</t>
+        </is>
+      </c>
+      <c r="D20" s="6" t="inlineStr"/>
+      <c r="E20" s="6" t="inlineStr"/>
+      <c r="F20" s="6" t="inlineStr"/>
+      <c r="G20" s="6" t="inlineStr"/>
+      <c r="H20" s="6" t="inlineStr"/>
+      <c r="I20" s="6" t="inlineStr"/>
+      <c r="J20" s="6" t="inlineStr">
+        <is>
+          <t>Colton</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="6" t="inlineStr">
+        <is>
+          <t>4-0436</t>
+        </is>
+      </c>
+      <c r="B21" s="6" t="inlineStr">
+        <is>
+          <t>Ei00L</t>
+        </is>
+      </c>
+      <c r="C21" s="6" t="inlineStr">
+        <is>
+          <t>Relaxation Room - on hold</t>
+        </is>
+      </c>
+      <c r="D21" s="6" t="inlineStr"/>
+      <c r="E21" s="6" t="inlineStr"/>
+      <c r="F21" s="6" t="inlineStr"/>
+      <c r="G21" s="6" t="inlineStr"/>
+      <c r="H21" s="6" t="inlineStr"/>
+      <c r="I21" s="6" t="inlineStr"/>
+      <c r="J21" s="6" t="inlineStr">
+        <is>
+          <t>Colton</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="6" t="inlineStr">
         <is>
           <t>4-0532</t>
         </is>
       </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>Ei005 MR6</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>Replace Steam Coil</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>5-0534</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>Ch04</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>Replace Iso Dmp; some night after 10 pm</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>3-0423</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>Ei005-MR1</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>Wet Filter DP's!</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>4-0114</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>EiPH</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>EFI Iso Dampers</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>4-0201</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>Ch01</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>Pipe/Device VAVs</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>4-0271</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>JB - Labor</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>Fix piping for North side F/S Dampers, Rough-In, Stat relocates</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>4-0272</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>JB - Material</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>Material Only</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>3-0435</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>PTI Vibration</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>JB S-105A, JB S-105B, Ei58, EiR8</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>4-0277</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>Ch005</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>FC + N2 Clean-up, wire valves, upgrade between VAV</t>
-        </is>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>4-0322</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>Ch01</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>Cx 9/26</t>
-        </is>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>4-0485</t>
-        </is>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>Ei005-67</t>
-        </is>
-      </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>Facilities Shot | Panel: Relocate/Writing</t>
-        </is>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>4-0499</t>
-        </is>
-      </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>Ei01-106A</t>
-        </is>
-      </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>Cx</t>
+      <c r="B22" s="6" t="inlineStr">
+        <is>
+          <t>Ei00S-MR6</t>
+        </is>
+      </c>
+      <c r="C22" s="6" t="inlineStr">
+        <is>
+          <t>Replace Steam Coil / Low Limits</t>
+        </is>
+      </c>
+      <c r="D22" s="6" t="inlineStr"/>
+      <c r="E22" s="6" t="inlineStr"/>
+      <c r="F22" s="6" t="inlineStr"/>
+      <c r="G22" s="6" t="inlineStr"/>
+      <c r="H22" s="6" t="inlineStr"/>
+      <c r="I22" s="6" t="inlineStr"/>
+      <c r="J22" s="6" t="inlineStr">
+        <is>
+          <t>Colton</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="6" t="inlineStr">
+        <is>
+          <t>5-XXXX</t>
+        </is>
+      </c>
+      <c r="B23" s="6" t="inlineStr">
+        <is>
+          <t>Ch00S-227</t>
+        </is>
+      </c>
+      <c r="C23" s="6" t="inlineStr">
+        <is>
+          <t>Vault G - 3 Cooling only VAVs</t>
+        </is>
+      </c>
+      <c r="D23" s="6" t="inlineStr"/>
+      <c r="E23" s="6" t="inlineStr"/>
+      <c r="F23" s="6" t="inlineStr"/>
+      <c r="G23" s="6" t="inlineStr"/>
+      <c r="H23" s="6" t="inlineStr">
+        <is>
+          <t>Submittal</t>
+        </is>
+      </c>
+      <c r="I23" s="6" t="inlineStr"/>
+      <c r="J23" s="6" t="inlineStr">
+        <is>
+          <t>Colton</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="6" t="inlineStr">
+        <is>
+          <t>3n53-0338</t>
+        </is>
+      </c>
+      <c r="B24" s="6" t="inlineStr">
+        <is>
+          <t>Ei00L</t>
+        </is>
+      </c>
+      <c r="C24" s="6" t="inlineStr">
+        <is>
+          <t>Data Center and Dock Cutovers</t>
+        </is>
+      </c>
+      <c r="D24" s="6" t="inlineStr"/>
+      <c r="E24" s="6" t="inlineStr"/>
+      <c r="F24" s="6" t="inlineStr"/>
+      <c r="G24" s="6" t="inlineStr">
+        <is>
+          <t>Data center and Dock Cutovers</t>
+        </is>
+      </c>
+      <c r="H24" s="6" t="inlineStr"/>
+      <c r="I24" s="6" t="inlineStr"/>
+      <c r="J24" s="6" t="inlineStr">
+        <is>
+          <t>Sagan</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="6" t="inlineStr">
+        <is>
+          <t>3n53-0335</t>
+        </is>
+      </c>
+      <c r="B25" s="6" t="inlineStr">
+        <is>
+          <t>Ei00S</t>
+        </is>
+      </c>
+      <c r="C25" s="6" t="inlineStr">
+        <is>
+          <t>Final Closeout</t>
+        </is>
+      </c>
+      <c r="D25" s="6" t="inlineStr"/>
+      <c r="E25" s="6" t="inlineStr"/>
+      <c r="F25" s="6" t="inlineStr"/>
+      <c r="G25" s="6" t="inlineStr">
+        <is>
+          <t>As Builts in panels, Green Labels</t>
+        </is>
+      </c>
+      <c r="H25" s="6" t="inlineStr"/>
+      <c r="I25" s="6" t="inlineStr"/>
+      <c r="J25" s="6" t="inlineStr">
+        <is>
+          <t>Sagan</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="6" t="inlineStr">
+        <is>
+          <t>3n53-0339</t>
+        </is>
+      </c>
+      <c r="B26" s="6" t="inlineStr">
+        <is>
+          <t>Cn02P</t>
+        </is>
+      </c>
+      <c r="C26" s="6" t="inlineStr">
+        <is>
+          <t>S-65 and 66 Cutovers</t>
+        </is>
+      </c>
+      <c r="D26" s="6" t="inlineStr"/>
+      <c r="E26" s="6" t="inlineStr"/>
+      <c r="F26" s="6" t="inlineStr"/>
+      <c r="G26" s="6" t="inlineStr">
+        <is>
+          <t>Final Closeout</t>
+        </is>
+      </c>
+      <c r="H26" s="6" t="inlineStr"/>
+      <c r="I26" s="6" t="inlineStr"/>
+      <c r="J26" s="6" t="inlineStr">
+        <is>
+          <t>Sagan</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="6" t="inlineStr">
+        <is>
+          <t>3n53-0344</t>
+        </is>
+      </c>
+      <c r="B27" s="6" t="inlineStr">
+        <is>
+          <t>Ch00S</t>
+        </is>
+      </c>
+      <c r="C27" s="6" t="inlineStr">
+        <is>
+          <t>Domestic Hot Water Pumps</t>
+        </is>
+      </c>
+      <c r="D27" s="6" t="inlineStr"/>
+      <c r="E27" s="6" t="inlineStr"/>
+      <c r="F27" s="6" t="inlineStr"/>
+      <c r="G27" s="6" t="inlineStr">
+        <is>
+          <t>Verify Final Closeout</t>
+        </is>
+      </c>
+      <c r="H27" s="6" t="inlineStr"/>
+      <c r="I27" s="6" t="inlineStr"/>
+      <c r="J27" s="6" t="inlineStr">
+        <is>
+          <t>Sagan</t>
         </is>
       </c>
     </row>

</xml_diff>